<commit_message>
Avances importantes en el uso del modelo de reconocimiento facial
</commit_message>
<xml_diff>
--- a/registro_miembros.xlsx
+++ b/registro_miembros.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,22 +461,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>asdas</t>
+          <t>Fer</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>12.123.131-3</t>
+          <t>12.424.777-5</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>/home/dante/Documentos/repositorio-git/MVINACAP/CCTV/fotos/12.123.131-3_foto.jpg</t>
+          <t>CCTV/fotos/12424777-5/12.424.777-5_foto.jpg</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>x12c3</t>
+          <t>123123</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -488,83 +488,29 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>locura</t>
+          <t>Elon Musk</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>12.123.131-3</t>
+          <t>12.123.123-1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>/home/dante/Documentos/repositorio-git/MVINACAP/CCTV/fotos/12.123.131-3_foto.jpg</t>
+          <t>CCTV/fotos/12123123-1/12.123.123-1_foto.jpg</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>x12c3</t>
-        </is>
-      </c>
+          <t>123123</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Estudiante</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>locura</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>13.131.144-3</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>/home/dante/Documentos/repositorio-git/MVINACAP/CCTV/fotos/13.131.144-3_foto.jpg</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>x12c3</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Estudiante</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>locura</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>12.123.131-3</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>/home/dante/Documentos/repositorio-git/MVINACAP/CCTV/fotos/12.123.131-3_foto.jpg</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>x12c3</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Estudiante</t>
+          <t>Docente</t>
         </is>
       </c>
     </row>

</xml_diff>